<commit_message>
addition for positive BrobInts works
</commit_message>
<xml_diff>
--- a/assignment06/Grading Template 05.xlsx
+++ b/assignment06/Grading Template 05.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aavol\Documents\GitHub\aavolo\cmsi186\spring19\assignment05\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmyeh\Documents\College\Programming Lab\GitHub\cmsi186\assignment06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD0C1EF-535D-41FF-B931-C9734FEC0885}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDBFD4B3-22C8-45C7-92E2-8BAE1ABF4C32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="30220" windowHeight="19620" activeTab="6" xr2:uid="{63A3425B-6033-479B-8BF1-9D375DE2499F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{63A3425B-6033-479B-8BF1-9D375DE2499F}"/>
   </bookViews>
   <sheets>
     <sheet name="assignment00" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -727,7 +729,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -812,6 +814,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -824,20 +838,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1160,17 +1177,17 @@
       <selection activeCell="C18" sqref="C18:G34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="37" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
@@ -1184,7 +1201,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>1</v>
       </c>
@@ -1195,7 +1212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>2</v>
       </c>
@@ -1206,7 +1223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>3</v>
       </c>
@@ -1217,7 +1234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
         <v>4</v>
       </c>
@@ -1229,7 +1246,7 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C8" s="5" t="s">
         <v>14</v>
       </c>
@@ -1256,19 +1273,19 @@
       <selection activeCell="B3" sqref="B3:C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="62.90625" customWidth="1"/>
-    <col min="4" max="4" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
@@ -1282,7 +1299,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>1</v>
       </c>
@@ -1293,7 +1310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>2</v>
       </c>
@@ -1304,7 +1321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>3</v>
       </c>
@@ -1315,7 +1332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>4</v>
       </c>
@@ -1326,7 +1343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>5</v>
       </c>
@@ -1337,7 +1354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <v>6</v>
       </c>
@@ -1348,7 +1365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <v>7</v>
       </c>
@@ -1359,7 +1376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <v>8</v>
       </c>
@@ -1370,7 +1387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <v>9</v>
       </c>
@@ -1381,7 +1398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
         <v>10</v>
       </c>
@@ -1392,7 +1409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
         <v>11</v>
       </c>
@@ -1403,7 +1420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="4">
         <v>12</v>
       </c>
@@ -1415,7 +1432,7 @@
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C16" s="5" t="s">
         <v>14</v>
       </c>
@@ -1442,24 +1459,24 @@
       <selection activeCell="E33" sqref="E33:F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.6328125" customWidth="1"/>
-    <col min="4" max="4" width="35.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.54296875" style="12" customWidth="1"/>
-    <col min="6" max="6" width="12.36328125" customWidth="1"/>
-    <col min="9" max="9" width="20.90625" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="12" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="20.85546875" customWidth="1"/>
     <col min="11" max="11" width="40" customWidth="1"/>
-    <col min="12" max="12" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="11"/>
       <c r="C3" s="11" t="s">
         <v>0</v>
@@ -1474,8 +1491,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B4" s="36" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="40" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="2">
@@ -1488,8 +1505,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B5" s="36"/>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="40"/>
       <c r="C5" s="2">
         <v>2</v>
       </c>
@@ -1500,8 +1517,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B6" s="36"/>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="40"/>
       <c r="C6" s="2">
         <v>3</v>
       </c>
@@ -1512,8 +1529,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B7" s="36"/>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="40"/>
       <c r="C7" s="2">
         <v>4</v>
       </c>
@@ -1524,8 +1541,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B8" s="36"/>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="40"/>
       <c r="C8" s="2">
         <v>5</v>
       </c>
@@ -1536,8 +1553,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B9" s="36"/>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="40"/>
       <c r="C9" s="2">
         <v>6</v>
       </c>
@@ -1548,8 +1565,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B10" s="36"/>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="40"/>
       <c r="C10" s="2">
         <v>7</v>
       </c>
@@ -1560,8 +1577,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B11" s="37"/>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="41"/>
       <c r="C11" s="6">
         <v>8</v>
       </c>
@@ -1573,8 +1590,8 @@
       </c>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B12" s="38" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="42" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="9">
@@ -1588,8 +1605,8 @@
       </c>
       <c r="F12" s="10"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B13" s="36"/>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="40"/>
       <c r="C13" s="2">
         <v>2</v>
       </c>
@@ -1600,8 +1617,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B14" s="36"/>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="40"/>
       <c r="C14" s="2">
         <v>3</v>
       </c>
@@ -1612,8 +1629,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B15" s="36"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="40"/>
       <c r="C15" s="2">
         <v>4</v>
       </c>
@@ -1624,8 +1641,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B16" s="36"/>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="40"/>
       <c r="C16" s="2">
         <v>5</v>
       </c>
@@ -1636,8 +1653,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B17" s="36"/>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="40"/>
       <c r="C17" s="2">
         <v>6</v>
       </c>
@@ -1648,8 +1665,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B18" s="36"/>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="40"/>
       <c r="C18" s="2">
         <v>7</v>
       </c>
@@ -1660,8 +1677,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B19" s="36"/>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="40"/>
       <c r="C19" s="2">
         <v>8</v>
       </c>
@@ -1672,8 +1689,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B20" s="36"/>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="40"/>
       <c r="C20" s="2">
         <v>9</v>
       </c>
@@ -1684,8 +1701,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B21" s="37"/>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="41"/>
       <c r="C21" s="6">
         <v>10</v>
       </c>
@@ -1697,8 +1714,8 @@
       </c>
       <c r="F21" s="7"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B22" s="38" t="s">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="42" t="s">
         <v>34</v>
       </c>
       <c r="C22" s="9">
@@ -1712,8 +1729,8 @@
       </c>
       <c r="F22" s="10"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B23" s="36"/>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="40"/>
       <c r="C23" s="2">
         <v>2</v>
       </c>
@@ -1724,8 +1741,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B24" s="36"/>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="40"/>
       <c r="C24" s="2">
         <v>3</v>
       </c>
@@ -1736,8 +1753,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B25" s="36"/>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="40"/>
       <c r="C25" s="2">
         <v>4</v>
       </c>
@@ -1748,8 +1765,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B26" s="36"/>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="40"/>
       <c r="C26" s="2">
         <v>5</v>
       </c>
@@ -1760,8 +1777,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B27" s="36"/>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="40"/>
       <c r="C27" s="2">
         <v>6</v>
       </c>
@@ -1772,8 +1789,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B28" s="36"/>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="40"/>
       <c r="C28" s="2">
         <v>7</v>
       </c>
@@ -1784,8 +1801,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B29" s="37"/>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="41"/>
       <c r="C29" s="6">
         <v>8</v>
       </c>
@@ -1797,7 +1814,7 @@
       </c>
       <c r="F29" s="7"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="8"/>
       <c r="C30" s="2">
         <v>1</v>
@@ -1809,7 +1826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="8"/>
       <c r="C31" s="2">
         <v>2</v>
@@ -1821,7 +1838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C32" s="2">
         <v>3</v>
       </c>
@@ -1833,7 +1850,7 @@
       </c>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="4:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="4:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D33" s="5" t="s">
         <v>14</v>
       </c>
@@ -1864,24 +1881,24 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.6328125" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" style="19"/>
-    <col min="4" max="4" width="74.7265625" style="20" customWidth="1"/>
-    <col min="5" max="6" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.90625" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="19"/>
+    <col min="4" max="4" width="74.7109375" style="20" customWidth="1"/>
+    <col min="5" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.85546875" customWidth="1"/>
     <col min="11" max="11" width="40" customWidth="1"/>
-    <col min="12" max="12" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
       <c r="C3" s="26" t="s">
         <v>0</v>
@@ -1896,8 +1913,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B4" s="36" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="40" t="s">
         <v>51</v>
       </c>
       <c r="C4" s="8">
@@ -1910,8 +1927,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B5" s="36"/>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="40"/>
       <c r="C5" s="8">
         <v>2</v>
       </c>
@@ -1922,8 +1939,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B6" s="36"/>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="40"/>
       <c r="C6" s="8">
         <v>3</v>
       </c>
@@ -1934,8 +1951,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B7" s="36"/>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="40"/>
       <c r="C7" s="8">
         <v>4</v>
       </c>
@@ -1946,8 +1963,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B8" s="36"/>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="40"/>
       <c r="C8" s="8">
         <v>5</v>
       </c>
@@ -1958,8 +1975,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B9" s="36"/>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="40"/>
       <c r="C9" s="8">
         <v>6</v>
       </c>
@@ -1970,8 +1987,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B10" s="36"/>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="40"/>
       <c r="C10" s="8">
         <v>7</v>
       </c>
@@ -1982,8 +1999,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B11" s="36"/>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="40"/>
       <c r="C11" s="8">
         <v>8</v>
       </c>
@@ -1994,8 +2011,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B12" s="38" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="42" t="s">
         <v>52</v>
       </c>
       <c r="C12" s="27">
@@ -2009,8 +2026,8 @@
       </c>
       <c r="F12" s="10"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B13" s="36"/>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="40"/>
       <c r="C13" s="8">
         <v>2</v>
       </c>
@@ -2021,8 +2038,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="B14" s="36"/>
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" s="40"/>
       <c r="C14" s="8">
         <v>3</v>
       </c>
@@ -2033,8 +2050,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B15" s="36"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="40"/>
       <c r="C15" s="8">
         <v>4</v>
       </c>
@@ -2045,8 +2062,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B16" s="36"/>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="40"/>
       <c r="C16" s="8">
         <v>5</v>
       </c>
@@ -2057,8 +2074,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B17" s="36"/>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="40"/>
       <c r="C17" s="8">
         <v>6</v>
       </c>
@@ -2069,8 +2086,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B18" s="36"/>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="40"/>
       <c r="C18" s="8">
         <v>7</v>
       </c>
@@ -2081,8 +2098,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B19" s="36"/>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="40"/>
       <c r="C19" s="8">
         <v>8</v>
       </c>
@@ -2093,8 +2110,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B20" s="37"/>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="41"/>
       <c r="C20" s="28">
         <v>9</v>
       </c>
@@ -2106,8 +2123,8 @@
       </c>
       <c r="F20" s="7"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B21" s="36" t="s">
+    <row r="21" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B21" s="40" t="s">
         <v>77</v>
       </c>
       <c r="C21" s="8">
@@ -2120,8 +2137,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="39"/>
+    <row r="22" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="43"/>
       <c r="C22" s="29">
         <v>2</v>
       </c>
@@ -2133,7 +2150,7 @@
       </c>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D23" s="24" t="s">
         <v>14</v>
       </c>
@@ -2164,25 +2181,25 @@
       <selection activeCell="F4" sqref="F4:F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.6328125" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" style="19"/>
-    <col min="4" max="4" width="93.54296875" style="20" customWidth="1"/>
-    <col min="5" max="5" width="13.453125" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.36328125" customWidth="1"/>
-    <col min="9" max="9" width="20.90625" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="19"/>
+    <col min="4" max="4" width="93.5703125" style="20" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" customWidth="1"/>
+    <col min="9" max="9" width="20.85546875" customWidth="1"/>
     <col min="11" max="11" width="40" customWidth="1"/>
-    <col min="12" max="12" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
       <c r="C3" s="26" t="s">
         <v>0</v>
@@ -2197,8 +2214,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B4" s="36" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="40" t="s">
         <v>51</v>
       </c>
       <c r="C4" s="8">
@@ -2211,8 +2228,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B5" s="36"/>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="40"/>
       <c r="C5" s="8">
         <v>2</v>
       </c>
@@ -2223,8 +2240,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B6" s="36"/>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="40"/>
       <c r="C6" s="8">
         <v>3</v>
       </c>
@@ -2235,8 +2252,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B7" s="38" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="42" t="s">
         <v>89</v>
       </c>
       <c r="C7" s="27">
@@ -2250,8 +2267,8 @@
       </c>
       <c r="F7" s="10"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B8" s="36"/>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="40"/>
       <c r="C8" s="8">
         <v>2</v>
       </c>
@@ -2262,8 +2279,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B9" s="36"/>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="40"/>
       <c r="C9" s="8">
         <v>3</v>
       </c>
@@ -2274,8 +2291,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B10" s="36"/>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="40"/>
       <c r="C10" s="8">
         <v>4</v>
       </c>
@@ -2286,8 +2303,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B11" s="36"/>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="40"/>
       <c r="C11" s="8">
         <v>5</v>
       </c>
@@ -2298,8 +2315,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B12" s="37"/>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="41"/>
       <c r="C12" s="28">
         <v>6</v>
       </c>
@@ -2311,8 +2328,8 @@
       </c>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B13" s="38" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="42" t="s">
         <v>90</v>
       </c>
       <c r="C13" s="27">
@@ -2326,8 +2343,8 @@
       </c>
       <c r="F13" s="10"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B14" s="36"/>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="40"/>
       <c r="C14" s="8">
         <v>2</v>
       </c>
@@ -2338,8 +2355,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B15" s="36"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="40"/>
       <c r="C15" s="19">
         <v>3</v>
       </c>
@@ -2350,8 +2367,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B16" s="36"/>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="40"/>
       <c r="C16" s="8">
         <v>4</v>
       </c>
@@ -2362,8 +2379,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B17" s="36"/>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="40"/>
       <c r="C17" s="8">
         <v>5</v>
       </c>
@@ -2374,8 +2391,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B18" s="36"/>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="40"/>
       <c r="C18" s="8">
         <v>6</v>
       </c>
@@ -2386,8 +2403,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B19" s="36"/>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="40"/>
       <c r="C19" s="8">
         <v>7</v>
       </c>
@@ -2398,8 +2415,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B20" s="36"/>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="40"/>
       <c r="C20" s="8">
         <v>8</v>
       </c>
@@ -2410,8 +2427,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B21" s="36"/>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="40"/>
       <c r="C21" s="8">
         <v>9</v>
       </c>
@@ -2422,8 +2439,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B22" s="36"/>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="40"/>
       <c r="C22" s="8">
         <v>10</v>
       </c>
@@ -2434,8 +2451,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B23" s="36"/>
+    <row r="23" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B23" s="40"/>
       <c r="C23" s="8">
         <v>11</v>
       </c>
@@ -2446,8 +2463,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B24" s="36"/>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="40"/>
       <c r="C24" s="8">
         <v>12</v>
       </c>
@@ -2458,8 +2475,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B25" s="37"/>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="41"/>
       <c r="C25" s="28">
         <v>13</v>
       </c>
@@ -2471,8 +2488,8 @@
       </c>
       <c r="F25" s="7"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B26" s="38" t="s">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="42" t="s">
         <v>77</v>
       </c>
       <c r="C26" s="27">
@@ -2486,8 +2503,8 @@
       </c>
       <c r="F26" s="10"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B27" s="37"/>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="41"/>
       <c r="C27" s="28">
         <v>2</v>
       </c>
@@ -2499,8 +2516,8 @@
       </c>
       <c r="F27" s="7"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B28" s="36" t="s">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="40" t="s">
         <v>97</v>
       </c>
       <c r="C28" s="8">
@@ -2513,8 +2530,8 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B29" s="36"/>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="40"/>
       <c r="C29" s="8">
         <v>2</v>
       </c>
@@ -2525,8 +2542,8 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B30" s="36"/>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="40"/>
       <c r="C30" s="8">
         <v>3</v>
       </c>
@@ -2537,14 +2554,14 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B31" s="39"/>
+    <row r="31" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="43"/>
       <c r="C31" s="29"/>
       <c r="D31" s="25"/>
       <c r="E31" s="15"/>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D32" s="24" t="s">
         <v>14</v>
       </c>
@@ -2573,25 +2590,25 @@
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.6328125" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" style="19"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="19"/>
     <col min="4" max="4" width="103" style="20" customWidth="1"/>
-    <col min="5" max="5" width="13.453125" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.36328125" style="12" customWidth="1"/>
-    <col min="9" max="9" width="20.90625" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" style="12" customWidth="1"/>
+    <col min="9" max="9" width="20.85546875" customWidth="1"/>
     <col min="11" max="11" width="40" customWidth="1"/>
-    <col min="12" max="12" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
       <c r="C3" s="26" t="s">
         <v>0</v>
@@ -2606,8 +2623,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B4" s="36" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="40" t="s">
         <v>115</v>
       </c>
       <c r="C4" s="8"/>
@@ -2618,8 +2635,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B5" s="37"/>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="41"/>
       <c r="C5" s="28"/>
       <c r="D5" s="22" t="s">
         <v>117</v>
@@ -2629,8 +2646,8 @@
       </c>
       <c r="F5" s="14"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B6" s="38" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="42" t="s">
         <v>138</v>
       </c>
       <c r="C6" s="27"/>
@@ -2642,8 +2659,8 @@
       </c>
       <c r="F6" s="13"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B7" s="36"/>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="40"/>
       <c r="C7" s="8"/>
       <c r="D7" s="20" t="s">
         <v>124</v>
@@ -2652,8 +2669,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B8" s="36"/>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="40"/>
       <c r="C8" s="8"/>
       <c r="D8" s="20" t="s">
         <v>142</v>
@@ -2662,8 +2679,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B9" s="37"/>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="41"/>
       <c r="C9" s="28"/>
       <c r="D9" s="22" t="s">
         <v>141</v>
@@ -2673,8 +2690,8 @@
       </c>
       <c r="F9" s="14"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B10" s="38" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="42" t="s">
         <v>134</v>
       </c>
       <c r="C10" s="32"/>
@@ -2686,8 +2703,8 @@
       </c>
       <c r="F10" s="13"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B11" s="36"/>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="40"/>
       <c r="C11" s="8"/>
       <c r="D11" s="20" t="s">
         <v>126</v>
@@ -2696,8 +2713,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B12" s="36"/>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="40"/>
       <c r="C12" s="8"/>
       <c r="D12" s="20" t="s">
         <v>129</v>
@@ -2706,8 +2723,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B13" s="36"/>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="40"/>
       <c r="C13" s="8"/>
       <c r="D13" s="20" t="s">
         <v>131</v>
@@ -2716,8 +2733,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B14" s="36"/>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="40"/>
       <c r="C14" s="8"/>
       <c r="D14" s="20" t="s">
         <v>130</v>
@@ -2726,8 +2743,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B15" s="36"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="40"/>
       <c r="C15" s="8"/>
       <c r="D15" s="20" t="s">
         <v>132</v>
@@ -2736,8 +2753,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B16" s="36"/>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="40"/>
       <c r="C16" s="8"/>
       <c r="D16" s="20" t="s">
         <v>150</v>
@@ -2746,8 +2763,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B17" s="37"/>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="41"/>
       <c r="C17" s="28"/>
       <c r="D17" s="22" t="s">
         <v>145</v>
@@ -2757,8 +2774,8 @@
       </c>
       <c r="F17" s="14"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B18" s="38" t="s">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="42" t="s">
         <v>135</v>
       </c>
       <c r="C18" s="27"/>
@@ -2770,8 +2787,8 @@
       </c>
       <c r="F18" s="13"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B19" s="36"/>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="40"/>
       <c r="C19" s="8"/>
       <c r="D19" s="20" t="s">
         <v>144</v>
@@ -2780,8 +2797,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B20" s="36"/>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="40"/>
       <c r="C20" s="8"/>
       <c r="D20" s="20" t="s">
         <v>148</v>
@@ -2790,8 +2807,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B21" s="36"/>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="40"/>
       <c r="C21" s="8"/>
       <c r="D21" s="20" t="s">
         <v>149</v>
@@ -2800,8 +2817,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B22" s="37"/>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="41"/>
       <c r="C22" s="28"/>
       <c r="D22" s="22" t="s">
         <v>146</v>
@@ -2811,8 +2828,8 @@
       </c>
       <c r="F22" s="14"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B23" s="38" t="s">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="42" t="s">
         <v>136</v>
       </c>
       <c r="C23" s="27"/>
@@ -2824,8 +2841,8 @@
       </c>
       <c r="F23" s="13"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B24" s="37"/>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="41"/>
       <c r="C24" s="28"/>
       <c r="D24" s="22" t="s">
         <v>128</v>
@@ -2835,8 +2852,8 @@
       </c>
       <c r="F24" s="14"/>
     </row>
-    <row r="25" spans="2:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="B25" s="38" t="s">
+    <row r="25" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B25" s="42" t="s">
         <v>137</v>
       </c>
       <c r="C25" s="27"/>
@@ -2848,8 +2865,8 @@
       </c>
       <c r="F25" s="13"/>
     </row>
-    <row r="26" spans="2:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="B26" s="36"/>
+    <row r="26" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B26" s="40"/>
       <c r="C26" s="8"/>
       <c r="D26" s="20" t="s">
         <v>140</v>
@@ -2858,8 +2875,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B27" s="36"/>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="40"/>
       <c r="C27" s="8"/>
       <c r="D27" s="20" t="s">
         <v>139</v>
@@ -2868,8 +2885,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B28" s="36"/>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="40"/>
       <c r="C28" s="8"/>
       <c r="D28" s="20" t="s">
         <v>122</v>
@@ -2878,8 +2895,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B29" s="36"/>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="40"/>
       <c r="C29" s="8"/>
       <c r="D29" s="20" t="s">
         <v>121</v>
@@ -2888,8 +2905,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B30" s="36"/>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="40"/>
       <c r="C30" s="8"/>
       <c r="D30" s="20" t="s">
         <v>119</v>
@@ -2898,8 +2915,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="B31" s="37"/>
+    <row r="31" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B31" s="41"/>
       <c r="C31" s="28"/>
       <c r="D31" s="22" t="s">
         <v>120</v>
@@ -2909,8 +2926,8 @@
       </c>
       <c r="F31" s="14"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B32" s="36" t="s">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="40" t="s">
         <v>77</v>
       </c>
       <c r="C32" s="8"/>
@@ -2921,8 +2938,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B33" s="36"/>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="40"/>
       <c r="C33" s="8"/>
       <c r="D33" s="20" t="s">
         <v>87</v>
@@ -2931,8 +2948,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B34" s="37"/>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="41"/>
       <c r="C34" s="28"/>
       <c r="D34" s="22" t="s">
         <v>118</v>
@@ -2942,8 +2959,8 @@
       </c>
       <c r="F34" s="14"/>
     </row>
-    <row r="35" spans="2:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="B35" s="36" t="s">
+    <row r="35" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B35" s="40" t="s">
         <v>97</v>
       </c>
       <c r="C35" s="8"/>
@@ -2951,22 +2968,22 @@
         <v>147</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B36" s="36"/>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="40"/>
       <c r="C36" s="8"/>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B37" s="36"/>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="40"/>
       <c r="C37" s="8"/>
     </row>
-    <row r="38" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B38" s="39"/>
+    <row r="38" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="43"/>
       <c r="C38" s="29"/>
       <c r="D38" s="25"/>
       <c r="E38" s="15"/>
       <c r="F38" s="15"/>
     </row>
-    <row r="39" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D39" s="24" t="s">
         <v>14</v>
       </c>
@@ -2995,29 +3012,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21DF255E-8C45-4C79-AB9F-F1083B20A474}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="117" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.6328125" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" style="19"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="19"/>
     <col min="4" max="4" width="103" style="20" customWidth="1"/>
-    <col min="5" max="5" width="13.453125" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.36328125" style="12" customWidth="1"/>
-    <col min="9" max="9" width="20.90625" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" style="12" customWidth="1"/>
+    <col min="9" max="9" width="20.85546875" customWidth="1"/>
     <col min="11" max="11" width="40" customWidth="1"/>
-    <col min="12" max="12" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
       <c r="C3" s="26" t="s">
         <v>0</v>
@@ -3032,7 +3049,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" s="44" t="s">
         <v>151</v>
       </c>
@@ -3043,9 +3060,11 @@
       <c r="E4" s="35">
         <v>1</v>
       </c>
-      <c r="F4" s="35"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F4" s="45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="44"/>
       <c r="C5" s="33"/>
       <c r="D5" s="34" t="s">
@@ -3054,9 +3073,11 @@
       <c r="E5" s="35">
         <v>2</v>
       </c>
-      <c r="F5" s="35"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F5" s="45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" s="44"/>
       <c r="C6" s="33"/>
       <c r="D6" s="34" t="s">
@@ -3065,9 +3086,11 @@
       <c r="E6" s="35">
         <v>8</v>
       </c>
-      <c r="F6" s="35"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F6" s="45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" s="44"/>
       <c r="C7" s="33"/>
       <c r="D7" s="34" t="s">
@@ -3076,9 +3099,11 @@
       <c r="E7" s="35">
         <v>8</v>
       </c>
-      <c r="F7" s="35"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F7" s="45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="44"/>
       <c r="C8" s="33"/>
       <c r="D8" s="34" t="s">
@@ -3087,9 +3112,11 @@
       <c r="E8" s="35">
         <v>8</v>
       </c>
-      <c r="F8" s="35"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F8" s="45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="44"/>
       <c r="C9" s="33"/>
       <c r="D9" s="34" t="s">
@@ -3098,9 +3125,11 @@
       <c r="E9" s="35">
         <v>8</v>
       </c>
-      <c r="F9" s="35"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F9" s="45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" s="44"/>
       <c r="C10" s="33"/>
       <c r="D10" s="34" t="s">
@@ -3109,9 +3138,11 @@
       <c r="E10" s="35">
         <v>8</v>
       </c>
-      <c r="F10" s="34"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F10" s="49">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="44"/>
       <c r="C11" s="33"/>
       <c r="D11" s="34" t="s">
@@ -3120,9 +3151,9 @@
       <c r="E11" s="35">
         <v>4</v>
       </c>
-      <c r="F11" s="35"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F11" s="45"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="44"/>
       <c r="C12" s="33"/>
       <c r="D12" s="34" t="s">
@@ -3131,10 +3162,10 @@
       <c r="E12" s="35">
         <v>4</v>
       </c>
-      <c r="F12" s="35"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B13" s="37"/>
+      <c r="F12" s="45"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="41"/>
       <c r="C13" s="28"/>
       <c r="D13" s="22" t="s">
         <v>167</v>
@@ -3142,10 +3173,10 @@
       <c r="E13" s="14">
         <v>4</v>
       </c>
-      <c r="F13" s="14"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B14" s="36" t="s">
+      <c r="F13" s="46"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="40" t="s">
         <v>152</v>
       </c>
       <c r="C14" s="8"/>
@@ -3155,9 +3186,10 @@
       <c r="E14" s="12">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B15" s="36"/>
+      <c r="F14" s="47"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="40"/>
       <c r="C15" s="8"/>
       <c r="D15" s="20" t="s">
         <v>156</v>
@@ -3165,9 +3197,10 @@
       <c r="E15" s="12">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B16" s="36"/>
+      <c r="F15" s="47"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="40"/>
       <c r="C16" s="8"/>
       <c r="D16" s="20" t="s">
         <v>160</v>
@@ -3175,9 +3208,10 @@
       <c r="E16" s="12">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B17" s="38" t="s">
+      <c r="F16" s="47"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="42" t="s">
         <v>157</v>
       </c>
       <c r="C17" s="27"/>
@@ -3187,10 +3221,12 @@
       <c r="E17" s="13">
         <v>5</v>
       </c>
-      <c r="F17" s="13"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B18" s="36"/>
+      <c r="F17" s="48">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="40"/>
       <c r="C18" s="8"/>
       <c r="D18" s="20" t="s">
         <v>159</v>
@@ -3198,9 +3234,12 @@
       <c r="E18" s="12">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B19" s="36"/>
+      <c r="F18" s="47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="40"/>
       <c r="C19" s="8"/>
       <c r="D19" s="20" t="s">
         <v>168</v>
@@ -3208,9 +3247,12 @@
       <c r="E19" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B20" s="36"/>
+      <c r="F19" s="47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="40"/>
       <c r="C20" s="8"/>
       <c r="D20" s="20" t="s">
         <v>169</v>
@@ -3218,9 +3260,12 @@
       <c r="E20" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B21" s="36"/>
+      <c r="F20" s="47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="40"/>
       <c r="C21" s="8"/>
       <c r="D21" s="20" t="s">
         <v>170</v>
@@ -3228,9 +3273,12 @@
       <c r="E21" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B22" s="36"/>
+      <c r="F21" s="47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="40"/>
       <c r="C22" s="8"/>
       <c r="D22" s="20" t="s">
         <v>171</v>
@@ -3238,9 +3286,12 @@
       <c r="E22" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B23" s="36"/>
+      <c r="F22" s="47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="40"/>
       <c r="C23" s="8"/>
       <c r="D23" s="20" t="s">
         <v>172</v>
@@ -3248,9 +3299,12 @@
       <c r="E23" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B24" s="36"/>
+      <c r="F23" s="47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="40"/>
       <c r="C24" s="8"/>
       <c r="D24" s="20" t="s">
         <v>173</v>
@@ -3258,9 +3312,12 @@
       <c r="E24" s="12">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B25" s="36"/>
+      <c r="F24" s="47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="40"/>
       <c r="C25" s="8"/>
       <c r="D25" s="20" t="s">
         <v>176</v>
@@ -3268,9 +3325,12 @@
       <c r="E25" s="12">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B26" s="36"/>
+      <c r="F25" s="47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="40"/>
       <c r="C26" s="8"/>
       <c r="D26" s="20" t="s">
         <v>139</v>
@@ -3278,9 +3338,12 @@
       <c r="E26" s="12">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="2:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="B27" s="38" t="s">
+      <c r="F26" s="47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B27" s="42" t="s">
         <v>77</v>
       </c>
       <c r="C27" s="27"/>
@@ -3290,9 +3353,9 @@
       <c r="E27" s="13">
         <v>3</v>
       </c>
-      <c r="F27" s="13"/>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F27" s="48"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="44"/>
       <c r="C28" s="33"/>
       <c r="D28" s="20" t="s">
@@ -3301,9 +3364,9 @@
       <c r="E28" s="35">
         <v>2</v>
       </c>
-      <c r="F28" s="35"/>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F28" s="45"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="44"/>
       <c r="C29" s="8"/>
       <c r="D29" s="20" t="s">
@@ -3312,8 +3375,9 @@
       <c r="E29" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F29" s="47"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="44"/>
       <c r="C30" s="8"/>
       <c r="D30" s="20" t="s">
@@ -3322,25 +3386,30 @@
       <c r="E30" s="12">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="2:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B31" s="40" t="s">
+      <c r="F30" s="47"/>
+    </row>
+    <row r="31" spans="2:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="C31" s="41"/>
-      <c r="D31" s="42" t="s">
+      <c r="C31" s="37"/>
+      <c r="D31" s="38" t="s">
         <v>175</v>
       </c>
-      <c r="E31" s="43"/>
-      <c r="F31" s="43"/>
-    </row>
-    <row r="32" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="E31" s="39"/>
+      <c r="F31" s="39"/>
+    </row>
+    <row r="32" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D32" s="24" t="s">
         <v>14</v>
       </c>
       <c r="E32" s="12">
         <f>SUM(E4:E30)</f>
         <v>100</v>
+      </c>
+      <c r="F32" s="12">
+        <f>SUM(F4:F30)</f>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -3366,18 +3435,18 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="32.1796875" customWidth="1"/>
-    <col min="4" max="4" width="18.08984375" customWidth="1"/>
-    <col min="5" max="5" width="15.453125" customWidth="1"/>
-    <col min="6" max="6" width="10.90625" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1" s="2"/>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
         <v>56</v>
       </c>
@@ -3398,7 +3467,7 @@
       </c>
       <c r="H3" s="12"/>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>58</v>
       </c>
@@ -3418,7 +3487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>59</v>
       </c>
@@ -3438,7 +3507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>60</v>
       </c>
@@ -3458,7 +3527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>61</v>
       </c>
@@ -3478,7 +3547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>62</v>
       </c>
@@ -3490,7 +3559,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>113</v>
       </c>
@@ -3509,7 +3578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>63</v>
       </c>
@@ -3521,7 +3590,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>64</v>
       </c>
@@ -3533,7 +3602,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>65</v>
       </c>
@@ -3545,7 +3614,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>66</v>
       </c>
@@ -3557,7 +3626,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="2:8" s="19" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:8" s="19" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="4" t="s">
         <v>55</v>
       </c>
@@ -3577,7 +3646,7 @@
       <c r="G14" s="1"/>
       <c r="H14"/>
     </row>
-    <row r="15" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
         <v>70</v>
       </c>
@@ -3594,24 +3663,24 @@
       <c r="G15" s="19"/>
       <c r="H15" s="19"/>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
     </row>
   </sheetData>
@@ -3630,18 +3699,18 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="32.1796875" customWidth="1"/>
-    <col min="4" max="4" width="18.08984375" customWidth="1"/>
-    <col min="5" max="5" width="15.453125" customWidth="1"/>
-    <col min="6" max="6" width="10.90625" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1" s="2"/>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
         <v>56</v>
       </c>
@@ -3662,7 +3731,7 @@
       </c>
       <c r="H3" s="12"/>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>58</v>
       </c>
@@ -3681,7 +3750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>59</v>
       </c>
@@ -3700,7 +3769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>60</v>
       </c>
@@ -3719,7 +3788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>61</v>
       </c>
@@ -3738,7 +3807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>62</v>
       </c>
@@ -3750,7 +3819,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>63</v>
       </c>
@@ -3762,7 +3831,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>64</v>
       </c>
@@ -3774,7 +3843,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>65</v>
       </c>
@@ -3786,7 +3855,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>66</v>
       </c>
@@ -3798,7 +3867,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="2:8" s="19" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:8" s="19" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="4" t="s">
         <v>55</v>
       </c>
@@ -3818,7 +3887,7 @@
       <c r="G13" s="1"/>
       <c r="H13"/>
     </row>
-    <row r="14" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="s">
         <v>70</v>
       </c>
@@ -3835,19 +3904,19 @@
       <c r="G14" s="19"/>
       <c r="H14" s="19"/>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rest of functions except remainder
</commit_message>
<xml_diff>
--- a/assignment06/Grading Template 05.xlsx
+++ b/assignment06/Grading Template 05.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmyeh\Documents\College\Programming Lab\GitHub\cmsi186\assignment06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDBFD4B3-22C8-45C7-92E2-8BAE1ABF4C32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25F47B61-7987-4FE1-A1F5-60E5663D1251}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{63A3425B-6033-479B-8BF1-9D375DE2499F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{63A3425B-6033-479B-8BF1-9D375DE2499F}"/>
   </bookViews>
   <sheets>
     <sheet name="assignment00" sheetId="3" r:id="rId1"/>
@@ -826,6 +826,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -840,21 +855,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1492,7 +1492,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="45" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="2">
@@ -1506,7 +1506,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="40"/>
+      <c r="B5" s="45"/>
       <c r="C5" s="2">
         <v>2</v>
       </c>
@@ -1518,7 +1518,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="40"/>
+      <c r="B6" s="45"/>
       <c r="C6" s="2">
         <v>3</v>
       </c>
@@ -1530,7 +1530,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="40"/>
+      <c r="B7" s="45"/>
       <c r="C7" s="2">
         <v>4</v>
       </c>
@@ -1542,7 +1542,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="40"/>
+      <c r="B8" s="45"/>
       <c r="C8" s="2">
         <v>5</v>
       </c>
@@ -1554,7 +1554,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="40"/>
+      <c r="B9" s="45"/>
       <c r="C9" s="2">
         <v>6</v>
       </c>
@@ -1566,7 +1566,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="40"/>
+      <c r="B10" s="45"/>
       <c r="C10" s="2">
         <v>7</v>
       </c>
@@ -1578,7 +1578,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="41"/>
+      <c r="B11" s="46"/>
       <c r="C11" s="6">
         <v>8</v>
       </c>
@@ -1591,7 +1591,7 @@
       <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="47" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="9">
@@ -1606,7 +1606,7 @@
       <c r="F12" s="10"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="40"/>
+      <c r="B13" s="45"/>
       <c r="C13" s="2">
         <v>2</v>
       </c>
@@ -1618,7 +1618,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="40"/>
+      <c r="B14" s="45"/>
       <c r="C14" s="2">
         <v>3</v>
       </c>
@@ -1630,7 +1630,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="40"/>
+      <c r="B15" s="45"/>
       <c r="C15" s="2">
         <v>4</v>
       </c>
@@ -1642,7 +1642,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="40"/>
+      <c r="B16" s="45"/>
       <c r="C16" s="2">
         <v>5</v>
       </c>
@@ -1654,7 +1654,7 @@
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="40"/>
+      <c r="B17" s="45"/>
       <c r="C17" s="2">
         <v>6</v>
       </c>
@@ -1666,7 +1666,7 @@
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="40"/>
+      <c r="B18" s="45"/>
       <c r="C18" s="2">
         <v>7</v>
       </c>
@@ -1678,7 +1678,7 @@
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="40"/>
+      <c r="B19" s="45"/>
       <c r="C19" s="2">
         <v>8</v>
       </c>
@@ -1690,7 +1690,7 @@
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="40"/>
+      <c r="B20" s="45"/>
       <c r="C20" s="2">
         <v>9</v>
       </c>
@@ -1702,7 +1702,7 @@
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="41"/>
+      <c r="B21" s="46"/>
       <c r="C21" s="6">
         <v>10</v>
       </c>
@@ -1715,7 +1715,7 @@
       <c r="F21" s="7"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="42" t="s">
+      <c r="B22" s="47" t="s">
         <v>34</v>
       </c>
       <c r="C22" s="9">
@@ -1730,7 +1730,7 @@
       <c r="F22" s="10"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="40"/>
+      <c r="B23" s="45"/>
       <c r="C23" s="2">
         <v>2</v>
       </c>
@@ -1742,7 +1742,7 @@
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="40"/>
+      <c r="B24" s="45"/>
       <c r="C24" s="2">
         <v>3</v>
       </c>
@@ -1754,7 +1754,7 @@
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="40"/>
+      <c r="B25" s="45"/>
       <c r="C25" s="2">
         <v>4</v>
       </c>
@@ -1766,7 +1766,7 @@
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="40"/>
+      <c r="B26" s="45"/>
       <c r="C26" s="2">
         <v>5</v>
       </c>
@@ -1778,7 +1778,7 @@
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="40"/>
+      <c r="B27" s="45"/>
       <c r="C27" s="2">
         <v>6</v>
       </c>
@@ -1790,7 +1790,7 @@
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="40"/>
+      <c r="B28" s="45"/>
       <c r="C28" s="2">
         <v>7</v>
       </c>
@@ -1802,7 +1802,7 @@
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="41"/>
+      <c r="B29" s="46"/>
       <c r="C29" s="6">
         <v>8</v>
       </c>
@@ -1914,7 +1914,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="45" t="s">
         <v>51</v>
       </c>
       <c r="C4" s="8">
@@ -1928,7 +1928,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="40"/>
+      <c r="B5" s="45"/>
       <c r="C5" s="8">
         <v>2</v>
       </c>
@@ -1940,7 +1940,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="40"/>
+      <c r="B6" s="45"/>
       <c r="C6" s="8">
         <v>3</v>
       </c>
@@ -1952,7 +1952,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="40"/>
+      <c r="B7" s="45"/>
       <c r="C7" s="8">
         <v>4</v>
       </c>
@@ -1964,7 +1964,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="40"/>
+      <c r="B8" s="45"/>
       <c r="C8" s="8">
         <v>5</v>
       </c>
@@ -1976,7 +1976,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="40"/>
+      <c r="B9" s="45"/>
       <c r="C9" s="8">
         <v>6</v>
       </c>
@@ -1988,7 +1988,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="40"/>
+      <c r="B10" s="45"/>
       <c r="C10" s="8">
         <v>7</v>
       </c>
@@ -2000,7 +2000,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="40"/>
+      <c r="B11" s="45"/>
       <c r="C11" s="8">
         <v>8</v>
       </c>
@@ -2012,7 +2012,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="47" t="s">
         <v>52</v>
       </c>
       <c r="C12" s="27">
@@ -2027,7 +2027,7 @@
       <c r="F12" s="10"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="40"/>
+      <c r="B13" s="45"/>
       <c r="C13" s="8">
         <v>2</v>
       </c>
@@ -2039,7 +2039,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="40"/>
+      <c r="B14" s="45"/>
       <c r="C14" s="8">
         <v>3</v>
       </c>
@@ -2051,7 +2051,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="40"/>
+      <c r="B15" s="45"/>
       <c r="C15" s="8">
         <v>4</v>
       </c>
@@ -2063,7 +2063,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="40"/>
+      <c r="B16" s="45"/>
       <c r="C16" s="8">
         <v>5</v>
       </c>
@@ -2075,7 +2075,7 @@
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="40"/>
+      <c r="B17" s="45"/>
       <c r="C17" s="8">
         <v>6</v>
       </c>
@@ -2087,7 +2087,7 @@
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="40"/>
+      <c r="B18" s="45"/>
       <c r="C18" s="8">
         <v>7</v>
       </c>
@@ -2099,7 +2099,7 @@
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="40"/>
+      <c r="B19" s="45"/>
       <c r="C19" s="8">
         <v>8</v>
       </c>
@@ -2111,7 +2111,7 @@
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="41"/>
+      <c r="B20" s="46"/>
       <c r="C20" s="28">
         <v>9</v>
       </c>
@@ -2124,7 +2124,7 @@
       <c r="F20" s="7"/>
     </row>
     <row r="21" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B21" s="40" t="s">
+      <c r="B21" s="45" t="s">
         <v>77</v>
       </c>
       <c r="C21" s="8">
@@ -2138,7 +2138,7 @@
       </c>
     </row>
     <row r="22" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="43"/>
+      <c r="B22" s="48"/>
       <c r="C22" s="29">
         <v>2</v>
       </c>
@@ -2215,7 +2215,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="45" t="s">
         <v>51</v>
       </c>
       <c r="C4" s="8">
@@ -2229,7 +2229,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="40"/>
+      <c r="B5" s="45"/>
       <c r="C5" s="8">
         <v>2</v>
       </c>
@@ -2241,7 +2241,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="40"/>
+      <c r="B6" s="45"/>
       <c r="C6" s="8">
         <v>3</v>
       </c>
@@ -2253,7 +2253,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="47" t="s">
         <v>89</v>
       </c>
       <c r="C7" s="27">
@@ -2268,7 +2268,7 @@
       <c r="F7" s="10"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="40"/>
+      <c r="B8" s="45"/>
       <c r="C8" s="8">
         <v>2</v>
       </c>
@@ -2280,7 +2280,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="40"/>
+      <c r="B9" s="45"/>
       <c r="C9" s="8">
         <v>3</v>
       </c>
@@ -2292,7 +2292,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="40"/>
+      <c r="B10" s="45"/>
       <c r="C10" s="8">
         <v>4</v>
       </c>
@@ -2304,7 +2304,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="40"/>
+      <c r="B11" s="45"/>
       <c r="C11" s="8">
         <v>5</v>
       </c>
@@ -2316,7 +2316,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="41"/>
+      <c r="B12" s="46"/>
       <c r="C12" s="28">
         <v>6</v>
       </c>
@@ -2329,7 +2329,7 @@
       <c r="F12" s="7"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="42" t="s">
+      <c r="B13" s="47" t="s">
         <v>90</v>
       </c>
       <c r="C13" s="27">
@@ -2344,7 +2344,7 @@
       <c r="F13" s="10"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="40"/>
+      <c r="B14" s="45"/>
       <c r="C14" s="8">
         <v>2</v>
       </c>
@@ -2356,7 +2356,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="40"/>
+      <c r="B15" s="45"/>
       <c r="C15" s="19">
         <v>3</v>
       </c>
@@ -2368,7 +2368,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="40"/>
+      <c r="B16" s="45"/>
       <c r="C16" s="8">
         <v>4</v>
       </c>
@@ -2380,7 +2380,7 @@
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="40"/>
+      <c r="B17" s="45"/>
       <c r="C17" s="8">
         <v>5</v>
       </c>
@@ -2392,7 +2392,7 @@
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="40"/>
+      <c r="B18" s="45"/>
       <c r="C18" s="8">
         <v>6</v>
       </c>
@@ -2404,7 +2404,7 @@
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="40"/>
+      <c r="B19" s="45"/>
       <c r="C19" s="8">
         <v>7</v>
       </c>
@@ -2416,7 +2416,7 @@
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="40"/>
+      <c r="B20" s="45"/>
       <c r="C20" s="8">
         <v>8</v>
       </c>
@@ -2428,7 +2428,7 @@
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="40"/>
+      <c r="B21" s="45"/>
       <c r="C21" s="8">
         <v>9</v>
       </c>
@@ -2440,7 +2440,7 @@
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="40"/>
+      <c r="B22" s="45"/>
       <c r="C22" s="8">
         <v>10</v>
       </c>
@@ -2452,7 +2452,7 @@
       </c>
     </row>
     <row r="23" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B23" s="40"/>
+      <c r="B23" s="45"/>
       <c r="C23" s="8">
         <v>11</v>
       </c>
@@ -2464,7 +2464,7 @@
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="40"/>
+      <c r="B24" s="45"/>
       <c r="C24" s="8">
         <v>12</v>
       </c>
@@ -2476,7 +2476,7 @@
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="41"/>
+      <c r="B25" s="46"/>
       <c r="C25" s="28">
         <v>13</v>
       </c>
@@ -2489,7 +2489,7 @@
       <c r="F25" s="7"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="42" t="s">
+      <c r="B26" s="47" t="s">
         <v>77</v>
       </c>
       <c r="C26" s="27">
@@ -2504,7 +2504,7 @@
       <c r="F26" s="10"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="41"/>
+      <c r="B27" s="46"/>
       <c r="C27" s="28">
         <v>2</v>
       </c>
@@ -2517,7 +2517,7 @@
       <c r="F27" s="7"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="40" t="s">
+      <c r="B28" s="45" t="s">
         <v>97</v>
       </c>
       <c r="C28" s="8">
@@ -2531,7 +2531,7 @@
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="40"/>
+      <c r="B29" s="45"/>
       <c r="C29" s="8">
         <v>2</v>
       </c>
@@ -2543,7 +2543,7 @@
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="40"/>
+      <c r="B30" s="45"/>
       <c r="C30" s="8">
         <v>3</v>
       </c>
@@ -2555,7 +2555,7 @@
       </c>
     </row>
     <row r="31" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="43"/>
+      <c r="B31" s="48"/>
       <c r="C31" s="29"/>
       <c r="D31" s="25"/>
       <c r="E31" s="15"/>
@@ -2586,7 +2586,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D28CC476-C225-4613-BF2F-2EEAD2AB9D1F}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView topLeftCell="B3" zoomScale="117" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="117" workbookViewId="0">
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
@@ -2624,7 +2624,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="45" t="s">
         <v>115</v>
       </c>
       <c r="C4" s="8"/>
@@ -2636,7 +2636,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="41"/>
+      <c r="B5" s="46"/>
       <c r="C5" s="28"/>
       <c r="D5" s="22" t="s">
         <v>117</v>
@@ -2647,7 +2647,7 @@
       <c r="F5" s="14"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="47" t="s">
         <v>138</v>
       </c>
       <c r="C6" s="27"/>
@@ -2660,7 +2660,7 @@
       <c r="F6" s="13"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="40"/>
+      <c r="B7" s="45"/>
       <c r="C7" s="8"/>
       <c r="D7" s="20" t="s">
         <v>124</v>
@@ -2670,7 +2670,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="40"/>
+      <c r="B8" s="45"/>
       <c r="C8" s="8"/>
       <c r="D8" s="20" t="s">
         <v>142</v>
@@ -2680,7 +2680,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="41"/>
+      <c r="B9" s="46"/>
       <c r="C9" s="28"/>
       <c r="D9" s="22" t="s">
         <v>141</v>
@@ -2691,7 +2691,7 @@
       <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="47" t="s">
         <v>134</v>
       </c>
       <c r="C10" s="32"/>
@@ -2704,7 +2704,7 @@
       <c r="F10" s="13"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="40"/>
+      <c r="B11" s="45"/>
       <c r="C11" s="8"/>
       <c r="D11" s="20" t="s">
         <v>126</v>
@@ -2714,7 +2714,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="40"/>
+      <c r="B12" s="45"/>
       <c r="C12" s="8"/>
       <c r="D12" s="20" t="s">
         <v>129</v>
@@ -2724,7 +2724,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="40"/>
+      <c r="B13" s="45"/>
       <c r="C13" s="8"/>
       <c r="D13" s="20" t="s">
         <v>131</v>
@@ -2734,7 +2734,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="40"/>
+      <c r="B14" s="45"/>
       <c r="C14" s="8"/>
       <c r="D14" s="20" t="s">
         <v>130</v>
@@ -2744,7 +2744,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="40"/>
+      <c r="B15" s="45"/>
       <c r="C15" s="8"/>
       <c r="D15" s="20" t="s">
         <v>132</v>
@@ -2754,7 +2754,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="40"/>
+      <c r="B16" s="45"/>
       <c r="C16" s="8"/>
       <c r="D16" s="20" t="s">
         <v>150</v>
@@ -2764,7 +2764,7 @@
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="41"/>
+      <c r="B17" s="46"/>
       <c r="C17" s="28"/>
       <c r="D17" s="22" t="s">
         <v>145</v>
@@ -2775,7 +2775,7 @@
       <c r="F17" s="14"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="47" t="s">
         <v>135</v>
       </c>
       <c r="C18" s="27"/>
@@ -2788,7 +2788,7 @@
       <c r="F18" s="13"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="40"/>
+      <c r="B19" s="45"/>
       <c r="C19" s="8"/>
       <c r="D19" s="20" t="s">
         <v>144</v>
@@ -2798,7 +2798,7 @@
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="40"/>
+      <c r="B20" s="45"/>
       <c r="C20" s="8"/>
       <c r="D20" s="20" t="s">
         <v>148</v>
@@ -2808,7 +2808,7 @@
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="40"/>
+      <c r="B21" s="45"/>
       <c r="C21" s="8"/>
       <c r="D21" s="20" t="s">
         <v>149</v>
@@ -2818,7 +2818,7 @@
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="41"/>
+      <c r="B22" s="46"/>
       <c r="C22" s="28"/>
       <c r="D22" s="22" t="s">
         <v>146</v>
@@ -2829,7 +2829,7 @@
       <c r="F22" s="14"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="42" t="s">
+      <c r="B23" s="47" t="s">
         <v>136</v>
       </c>
       <c r="C23" s="27"/>
@@ -2842,7 +2842,7 @@
       <c r="F23" s="13"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="41"/>
+      <c r="B24" s="46"/>
       <c r="C24" s="28"/>
       <c r="D24" s="22" t="s">
         <v>128</v>
@@ -2853,7 +2853,7 @@
       <c r="F24" s="14"/>
     </row>
     <row r="25" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B25" s="42" t="s">
+      <c r="B25" s="47" t="s">
         <v>137</v>
       </c>
       <c r="C25" s="27"/>
@@ -2866,7 +2866,7 @@
       <c r="F25" s="13"/>
     </row>
     <row r="26" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B26" s="40"/>
+      <c r="B26" s="45"/>
       <c r="C26" s="8"/>
       <c r="D26" s="20" t="s">
         <v>140</v>
@@ -2876,7 +2876,7 @@
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="40"/>
+      <c r="B27" s="45"/>
       <c r="C27" s="8"/>
       <c r="D27" s="20" t="s">
         <v>139</v>
@@ -2886,7 +2886,7 @@
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="40"/>
+      <c r="B28" s="45"/>
       <c r="C28" s="8"/>
       <c r="D28" s="20" t="s">
         <v>122</v>
@@ -2896,7 +2896,7 @@
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="40"/>
+      <c r="B29" s="45"/>
       <c r="C29" s="8"/>
       <c r="D29" s="20" t="s">
         <v>121</v>
@@ -2906,7 +2906,7 @@
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="40"/>
+      <c r="B30" s="45"/>
       <c r="C30" s="8"/>
       <c r="D30" s="20" t="s">
         <v>119</v>
@@ -2916,7 +2916,7 @@
       </c>
     </row>
     <row r="31" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B31" s="41"/>
+      <c r="B31" s="46"/>
       <c r="C31" s="28"/>
       <c r="D31" s="22" t="s">
         <v>120</v>
@@ -2927,7 +2927,7 @@
       <c r="F31" s="14"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="40" t="s">
+      <c r="B32" s="45" t="s">
         <v>77</v>
       </c>
       <c r="C32" s="8"/>
@@ -2939,7 +2939,7 @@
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="40"/>
+      <c r="B33" s="45"/>
       <c r="C33" s="8"/>
       <c r="D33" s="20" t="s">
         <v>87</v>
@@ -2949,7 +2949,7 @@
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="41"/>
+      <c r="B34" s="46"/>
       <c r="C34" s="28"/>
       <c r="D34" s="22" t="s">
         <v>118</v>
@@ -2960,7 +2960,7 @@
       <c r="F34" s="14"/>
     </row>
     <row r="35" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B35" s="40" t="s">
+      <c r="B35" s="45" t="s">
         <v>97</v>
       </c>
       <c r="C35" s="8"/>
@@ -2969,15 +2969,15 @@
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="40"/>
+      <c r="B36" s="45"/>
       <c r="C36" s="8"/>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="40"/>
+      <c r="B37" s="45"/>
       <c r="C37" s="8"/>
     </row>
     <row r="38" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="43"/>
+      <c r="B38" s="48"/>
       <c r="C38" s="29"/>
       <c r="D38" s="25"/>
       <c r="E38" s="15"/>
@@ -3012,8 +3012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21DF255E-8C45-4C79-AB9F-F1083B20A474}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="117" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView topLeftCell="A4" zoomScale="117" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3050,7 +3050,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="49" t="s">
         <v>151</v>
       </c>
       <c r="C4" s="33"/>
@@ -3060,12 +3060,12 @@
       <c r="E4" s="35">
         <v>1</v>
       </c>
-      <c r="F4" s="45">
+      <c r="F4" s="40">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="44"/>
+      <c r="B5" s="49"/>
       <c r="C5" s="33"/>
       <c r="D5" s="34" t="s">
         <v>155</v>
@@ -3073,12 +3073,12 @@
       <c r="E5" s="35">
         <v>2</v>
       </c>
-      <c r="F5" s="45">
+      <c r="F5" s="40">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="44"/>
+      <c r="B6" s="49"/>
       <c r="C6" s="33"/>
       <c r="D6" s="34" t="s">
         <v>161</v>
@@ -3086,12 +3086,12 @@
       <c r="E6" s="35">
         <v>8</v>
       </c>
-      <c r="F6" s="45">
+      <c r="F6" s="40">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="44"/>
+      <c r="B7" s="49"/>
       <c r="C7" s="33"/>
       <c r="D7" s="34" t="s">
         <v>165</v>
@@ -3099,12 +3099,12 @@
       <c r="E7" s="35">
         <v>8</v>
       </c>
-      <c r="F7" s="45">
+      <c r="F7" s="40">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="44"/>
+      <c r="B8" s="49"/>
       <c r="C8" s="33"/>
       <c r="D8" s="34" t="s">
         <v>166</v>
@@ -3112,12 +3112,12 @@
       <c r="E8" s="35">
         <v>8</v>
       </c>
-      <c r="F8" s="45">
+      <c r="F8" s="40">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="44"/>
+      <c r="B9" s="49"/>
       <c r="C9" s="33"/>
       <c r="D9" s="34" t="s">
         <v>162</v>
@@ -3125,12 +3125,12 @@
       <c r="E9" s="35">
         <v>8</v>
       </c>
-      <c r="F9" s="45">
+      <c r="F9" s="40">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="44"/>
+      <c r="B10" s="49"/>
       <c r="C10" s="33"/>
       <c r="D10" s="34" t="s">
         <v>163</v>
@@ -3138,12 +3138,10 @@
       <c r="E10" s="35">
         <v>8</v>
       </c>
-      <c r="F10" s="49">
-        <v>8</v>
-      </c>
+      <c r="F10" s="44"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="44"/>
+      <c r="B11" s="49"/>
       <c r="C11" s="33"/>
       <c r="D11" s="34" t="s">
         <v>174</v>
@@ -3151,10 +3149,10 @@
       <c r="E11" s="35">
         <v>4</v>
       </c>
-      <c r="F11" s="45"/>
+      <c r="F11" s="40"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="44"/>
+      <c r="B12" s="49"/>
       <c r="C12" s="33"/>
       <c r="D12" s="34" t="s">
         <v>164</v>
@@ -3162,10 +3160,10 @@
       <c r="E12" s="35">
         <v>4</v>
       </c>
-      <c r="F12" s="45"/>
+      <c r="F12" s="40"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="41"/>
+      <c r="B13" s="46"/>
       <c r="C13" s="28"/>
       <c r="D13" s="22" t="s">
         <v>167</v>
@@ -3173,10 +3171,10 @@
       <c r="E13" s="14">
         <v>4</v>
       </c>
-      <c r="F13" s="46"/>
+      <c r="F13" s="41"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="45" t="s">
         <v>152</v>
       </c>
       <c r="C14" s="8"/>
@@ -3186,10 +3184,12 @@
       <c r="E14" s="12">
         <v>1</v>
       </c>
-      <c r="F14" s="47"/>
+      <c r="F14" s="42">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="40"/>
+      <c r="B15" s="45"/>
       <c r="C15" s="8"/>
       <c r="D15" s="20" t="s">
         <v>156</v>
@@ -3197,10 +3197,12 @@
       <c r="E15" s="12">
         <v>2</v>
       </c>
-      <c r="F15" s="47"/>
+      <c r="F15" s="42">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="40"/>
+      <c r="B16" s="45"/>
       <c r="C16" s="8"/>
       <c r="D16" s="20" t="s">
         <v>160</v>
@@ -3208,10 +3210,10 @@
       <c r="E16" s="12">
         <v>8</v>
       </c>
-      <c r="F16" s="47"/>
+      <c r="F16" s="42"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="47" t="s">
         <v>157</v>
       </c>
       <c r="C17" s="27"/>
@@ -3221,12 +3223,12 @@
       <c r="E17" s="13">
         <v>5</v>
       </c>
-      <c r="F17" s="48">
+      <c r="F17" s="43">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="40"/>
+      <c r="B18" s="45"/>
       <c r="C18" s="8"/>
       <c r="D18" s="20" t="s">
         <v>159</v>
@@ -3234,12 +3236,12 @@
       <c r="E18" s="12">
         <v>1</v>
       </c>
-      <c r="F18" s="47">
+      <c r="F18" s="42">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="40"/>
+      <c r="B19" s="45"/>
       <c r="C19" s="8"/>
       <c r="D19" s="20" t="s">
         <v>168</v>
@@ -3247,12 +3249,12 @@
       <c r="E19" s="12">
         <v>3</v>
       </c>
-      <c r="F19" s="47">
+      <c r="F19" s="42">
         <v>3</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="40"/>
+      <c r="B20" s="45"/>
       <c r="C20" s="8"/>
       <c r="D20" s="20" t="s">
         <v>169</v>
@@ -3260,12 +3262,12 @@
       <c r="E20" s="12">
         <v>3</v>
       </c>
-      <c r="F20" s="47">
+      <c r="F20" s="42">
         <v>3</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="40"/>
+      <c r="B21" s="45"/>
       <c r="C21" s="8"/>
       <c r="D21" s="20" t="s">
         <v>170</v>
@@ -3273,12 +3275,12 @@
       <c r="E21" s="12">
         <v>3</v>
       </c>
-      <c r="F21" s="47">
+      <c r="F21" s="42">
         <v>3</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="40"/>
+      <c r="B22" s="45"/>
       <c r="C22" s="8"/>
       <c r="D22" s="20" t="s">
         <v>171</v>
@@ -3286,12 +3288,12 @@
       <c r="E22" s="12">
         <v>3</v>
       </c>
-      <c r="F22" s="47">
+      <c r="F22" s="42">
         <v>3</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="40"/>
+      <c r="B23" s="45"/>
       <c r="C23" s="8"/>
       <c r="D23" s="20" t="s">
         <v>172</v>
@@ -3299,12 +3301,12 @@
       <c r="E23" s="12">
         <v>3</v>
       </c>
-      <c r="F23" s="47">
+      <c r="F23" s="42">
         <v>3</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="40"/>
+      <c r="B24" s="45"/>
       <c r="C24" s="8"/>
       <c r="D24" s="20" t="s">
         <v>173</v>
@@ -3312,12 +3314,12 @@
       <c r="E24" s="12">
         <v>1</v>
       </c>
-      <c r="F24" s="47">
+      <c r="F24" s="42">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="40"/>
+      <c r="B25" s="45"/>
       <c r="C25" s="8"/>
       <c r="D25" s="20" t="s">
         <v>176</v>
@@ -3325,12 +3327,12 @@
       <c r="E25" s="12">
         <v>2</v>
       </c>
-      <c r="F25" s="47">
+      <c r="F25" s="42">
         <v>2</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="40"/>
+      <c r="B26" s="45"/>
       <c r="C26" s="8"/>
       <c r="D26" s="20" t="s">
         <v>139</v>
@@ -3338,12 +3340,12 @@
       <c r="E26" s="12">
         <v>1</v>
       </c>
-      <c r="F26" s="47">
+      <c r="F26" s="42">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B27" s="42" t="s">
+      <c r="B27" s="47" t="s">
         <v>77</v>
       </c>
       <c r="C27" s="27"/>
@@ -3353,10 +3355,10 @@
       <c r="E27" s="13">
         <v>3</v>
       </c>
-      <c r="F27" s="48"/>
+      <c r="F27" s="43"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="44"/>
+      <c r="B28" s="49"/>
       <c r="C28" s="33"/>
       <c r="D28" s="20" t="s">
         <v>177</v>
@@ -3364,10 +3366,12 @@
       <c r="E28" s="35">
         <v>2</v>
       </c>
-      <c r="F28" s="45"/>
+      <c r="F28" s="40">
+        <v>2</v>
+      </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="44"/>
+      <c r="B29" s="49"/>
       <c r="C29" s="8"/>
       <c r="D29" s="20" t="s">
         <v>178</v>
@@ -3375,10 +3379,10 @@
       <c r="E29" s="12">
         <v>3</v>
       </c>
-      <c r="F29" s="47"/>
+      <c r="F29" s="42"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="44"/>
+      <c r="B30" s="49"/>
       <c r="C30" s="8"/>
       <c r="D30" s="20" t="s">
         <v>87</v>
@@ -3386,7 +3390,7 @@
       <c r="E30" s="12">
         <v>1</v>
       </c>
-      <c r="F30" s="47"/>
+      <c r="F30" s="42"/>
     </row>
     <row r="31" spans="2:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="36" t="s">
@@ -3409,7 +3413,7 @@
       </c>
       <c r="F32" s="12">
         <f>SUM(F4:F30)</f>
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -3432,7 +3436,7 @@
   <dimension ref="B1:H21"/>
   <sheetViews>
     <sheetView zoomScale="157" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3479,12 +3483,10 @@
         <v>4</v>
       </c>
       <c r="E4">
-        <f>assignment00!E8</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F4" s="16">
-        <f>IF(D4&lt;&gt;"",E4/D4,"")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -3658,7 +3660,7 @@
       <c r="E15" s="19"/>
       <c r="F15" s="30">
         <f>IF(F4&lt;&gt;"",F4*($C$4/$C$15),0)+IF(F5&lt;&gt;"",F5*($C$5/$C$15),0)+IF(F6&lt;&gt;"",F6*($C$6/$C$15),0)+IF(F7&lt;&gt;"",F7*($C$7/$C$15),0)+IF(F8&lt;&gt;"",F8*($C$8/$C$15),0)+IF(F10&lt;&gt;"",F10*($C$10/$C$15),0)+IF(F11&lt;&gt;"",F11*($C$11/$C$15),0)+IF(F12&lt;&gt;"",F12*($C$12/$C$15),0)+IF(F13&lt;&gt;"",F13*($C$13/$C$15),0)+IF(F14&lt;&gt;"",F14*($C$14/$C$15),0)+IF(F9&lt;&gt;"",F9*($C$9/$C$15),0)</f>
-        <v>0</v>
+        <v>0.14285714285714288</v>
       </c>
       <c r="G15" s="19"/>
       <c r="H15" s="19"/>
@@ -3696,7 +3698,7 @@
   <dimension ref="B1:H20"/>
   <sheetViews>
     <sheetView zoomScale="157" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C12" sqref="B11:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>